<commit_message>
refined code and data for weibull analysis. Filtered data from user dcb314.
</commit_message>
<xml_diff>
--- a/minix_test_data/github_data/marked.xlsx
+++ b/minix_test_data/github_data/marked.xlsx
@@ -364,7 +364,7 @@
   <dimension ref="A1:B135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,7 +971,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B76">
         <v>25</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B77">
         <v>24</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B79">
         <v>22</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B80">
         <v>21</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B81">
         <v>20</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B85">
         <v>16</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B133">
         <v>69</v>

</xml_diff>